<commit_message>
Manual evaluation COP22, COP22
</commit_message>
<xml_diff>
--- a/HLS_man/COP19/COP19_man_japan.xlsx
+++ b/HLS_man/COP19/COP19_man_japan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\Documents\GitHub\TextToDistributiveJustice\HLS_man\COP19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1880393-C8D2-49AF-9EF3-496901A89FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BE9DEB-D6AD-4603-8622-54E5104C8DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>COP19_japan</t>
   </si>
@@ -217,9 +217,6 @@
     <t>national</t>
   </si>
   <si>
-    <t>energy use</t>
-  </si>
-  <si>
     <t>sufficientarian</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t xml:space="preserve">
 As the next step, Japan has set a target to reduce emissions by 3.8 percent 
 compared to the 2005 level in 2020.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">policy target </t>
   </si>
   <si>
     <t>distant future</t>
@@ -684,23 +678,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.77734375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="67.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -729,7 +723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -737,7 +731,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -745,7 +739,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -753,7 +747,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -761,42 +755,42 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>40</v>
@@ -805,7 +799,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -813,7 +807,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -821,7 +815,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -829,23 +823,23 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" t="s">
         <v>42</v>
@@ -854,16 +848,16 @@
         <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
@@ -871,7 +865,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
@@ -879,33 +873,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
@@ -913,7 +889,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -921,7 +897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>19</v>
       </c>
@@ -929,7 +905,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>20</v>
       </c>
@@ -937,7 +913,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -948,7 +924,7 @@
       <c r="G19"/>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:9" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -956,7 +932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
@@ -964,7 +940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -972,7 +948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -980,7 +956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>26</v>
       </c>
@@ -988,7 +964,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="118.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>27</v>
       </c>
@@ -996,25 +972,25 @@
         <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1022,62 +998,62 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
         <v>37</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>39</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
         <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1085,7 +1061,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
@@ -1093,25 +1069,25 @@
         <v>37</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G30" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>31</v>
       </c>
@@ -1119,7 +1095,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>32</v>
       </c>
@@ -1127,7 +1103,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>33</v>
       </c>
@@ -1135,7 +1111,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Updated documents, Local folder file switch
</commit_message>
<xml_diff>
--- a/HLS_man/COP19/COP19_man_japan.xlsx
+++ b/HLS_man/COP19/COP19_man_japan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\Documents\GitHub\TextToDistributiveJustice\HLS_man\COP19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BE9DEB-D6AD-4603-8622-54E5104C8DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB34A062-010D-490B-BCD4-A9C1BA1A0763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>COP19_japan</t>
   </si>
@@ -202,39 +202,12 @@
     <t>global</t>
   </si>
   <si>
-    <t>utilitarian</t>
-  </si>
-  <si>
     <t>libertarian</t>
   </si>
   <si>
-    <t>national commitment</t>
-  </si>
-  <si>
-    <t>emissions</t>
-  </si>
-  <si>
-    <t>national</t>
-  </si>
-  <si>
-    <t>sufficientarian</t>
-  </si>
-  <si>
-    <t>general investment in relation to  "actions for a Cool Earth"</t>
-  </si>
-  <si>
-    <t>utilitarian, prioritarian</t>
-  </si>
-  <si>
     <t>prioritarian</t>
   </si>
   <si>
-    <t xml:space="preserve">Financial support of developing countries. </t>
-  </si>
-  <si>
-    <t>specific goals in global context</t>
-  </si>
-  <si>
     <t>new UNFCCC policy</t>
   </si>
   <si>
@@ -247,30 +220,7 @@
     <t>egalitarian</t>
   </si>
   <si>
-    <t>participation of all countries in taking measures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-In this regard, Japan firmly supports the establishment of a post-2020 
-framework. Such a framework must be based on “nationally -determined” commitment 
-and an effective international transparency mechanism.</t>
-  </si>
-  <si>
     <t>financial resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-First, Japan will promote further technological innovation . In this context, Japan’s public and private sectors plan to invest a total of 
-110 billion US dollars domestically over the next five years.</t>
-  </si>
-  <si>
-    <t>technological resources, financial resources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Our greenhouse gas emissions for the first commitme nt period is forecasted 
-to be 8.2 percent lower compared to the base year. As a result, our target under the Kyoto Protocol of 6 percent reduction has 
-been achieved.</t>
   </si>
   <si>
     <t>policy target</t>
@@ -286,27 +236,65 @@
 compared to the 2005 level in 2020.  </t>
   </si>
   <si>
-    <t>distant future</t>
-  </si>
-  <si>
-    <t>Second, Japan will promote the application of Japanese low-carbon. In so doing , we will contribute to global 
+    <t xml:space="preserve">n.a. </t>
+  </si>
+  <si>
+    <t>participation of all countries, reference to fairness</t>
+  </si>
+  <si>
+    <t>national commitment, minimizing the interference of a global institution leaving a country free to make own choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Our greenhouse gas emissions for the first commitme nt period is forecasted 
+to be 8.2 percent lower compared to the base year. </t>
+  </si>
+  <si>
+    <t>As a result, our target under the Kyoto Protocol of 6 percent reduction has 
+been achieved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+In this context, Japan’s public and private sectors plan to invest a total of 
+110 billion US dollars domestically over the next five years.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First, Japan will promote further technological innovation . </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In so doing , we will contribute to global 
 emission s reductions through the use of the Joint Crediting Mechanism, or 
 JCM .</t>
   </si>
   <si>
-    <t>link with previous sentence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JCM facilitaties decarboniation of partner countries, mostly non-annex1, making it prioritarian. Contributing to global emission reductions making it utilitarian. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.a. </t>
-  </si>
-  <si>
-    <t>other(JCM)</t>
-  </si>
-  <si>
-    <t>global, multinational(developed)</t>
+    <t>Second, Japan will promote the application of Japanese low-carbon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prescribing judgement about distribution of financial support to developing countries. </t>
+  </si>
+  <si>
+    <t>mitigation, adaptation</t>
+  </si>
+  <si>
+    <t>financial resources, other(assistance)</t>
+  </si>
+  <si>
+    <t>n.a.</t>
+  </si>
+  <si>
+    <t>general normative statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not applicable to a specific distribution, does imply value judgement on how resources should be distributed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+In this regard, Japan firmly supports the establishment of a post-2020 
+framework. </t>
+  </si>
+  <si>
+    <t>Such a framework must be based on “nationally -determined” commitment 
+and an effective international transparency mechanism.</t>
   </si>
 </sst>
 </file>
@@ -676,25 +664,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="67.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="67.88671875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -723,7 +711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -731,7 +719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -739,7 +727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -747,7 +735,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -755,367 +743,342 @@
         <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+    </row>
+    <row r="22" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" t="s">
+        <v>45</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="H34" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" t="s">
         <v>59</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19"/>
-      <c r="G19"/>
-      <c r="H19"/>
-    </row>
-    <row r="20" spans="1:9" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="118.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="H35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F27" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    </row>
+    <row r="36" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B38" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final man. annotated files
</commit_message>
<xml_diff>
--- a/HLS_man/COP19/COP19_man_japan.xlsx
+++ b/HLS_man/COP19/COP19_man_japan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\Documents\GitHub\TextToDistributiveJustice\HLS_man\COP19\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Suze van Santen\OneDrive - Delft University of Technology\Documenten\GitHub\TextToDistributiveJustice\HLS_man\COP19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB34A062-010D-490B-BCD4-A9C1BA1A0763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A359D08E-B558-4EAD-9BAB-C3DE48C6FD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>COP19_japan</t>
   </si>
@@ -44,19 +44,10 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Scale</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Principle</t>
   </si>
   <si>
     <t>30 word explanation</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t xml:space="preserve"> 
@@ -193,37 +184,10 @@
     <t>Topic</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>libertarian</t>
-  </si>
-  <si>
-    <t>prioritarian</t>
-  </si>
-  <si>
     <t>new UNFCCC policy</t>
   </si>
   <si>
-    <t>measures</t>
-  </si>
-  <si>
-    <t>nearby future</t>
-  </si>
-  <si>
     <t>egalitarian</t>
-  </si>
-  <si>
-    <t>financial resources</t>
-  </si>
-  <si>
-    <t>policy target</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -234,15 +198,6 @@
     <t xml:space="preserve">
 As the next step, Japan has set a target to reduce emissions by 3.8 percent 
 compared to the 2005 level in 2020.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">n.a. </t>
-  </si>
-  <si>
-    <t>participation of all countries, reference to fairness</t>
-  </si>
-  <si>
-    <t>national commitment, minimizing the interference of a global institution leaving a country free to make own choices</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -270,24 +225,6 @@
     <t>Second, Japan will promote the application of Japanese low-carbon.</t>
   </si>
   <si>
-    <t xml:space="preserve">Prescribing judgement about distribution of financial support to developing countries. </t>
-  </si>
-  <si>
-    <t>mitigation, adaptation</t>
-  </si>
-  <si>
-    <t>financial resources, other(assistance)</t>
-  </si>
-  <si>
-    <t>n.a.</t>
-  </si>
-  <si>
-    <t>general normative statement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">not applicable to a specific distribution, does imply value judgement on how resources should be distributed </t>
-  </si>
-  <si>
     <t xml:space="preserve">
 In this regard, Japan firmly supports the establishment of a post-2020 
 framework. </t>
@@ -295,13 +232,37 @@
   <si>
     <t>Such a framework must be based on “nationally -determined” commitment 
 and an effective international transparency mechanism.</t>
+  </si>
+  <si>
+    <t>responsibility</t>
+  </si>
+  <si>
+    <t>utilitarian</t>
+  </si>
+  <si>
+    <t>Shape</t>
+  </si>
+  <si>
+    <t>Motivation to reduce global emissions, need for a egalitarian distribution</t>
+  </si>
+  <si>
+    <t>Nationally determined refers to differentiation, aknowledging differences, indicating an egalitarian distribution</t>
+  </si>
+  <si>
+    <t>equality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equity </t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +275,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -351,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -362,6 +331,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -664,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="72" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -676,13 +646,12 @@
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="34.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="34.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -690,399 +659,354 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="127.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-    </row>
-    <row r="22" spans="1:8" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="118.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B35" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" t="s">
-        <v>59</v>
-      </c>
-      <c r="D35" t="s">
-        <v>60</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F35" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" t="s">
-        <v>36</v>
+      <c r="B38">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>